<commit_message>
CNBDOC Updated Tracker doc
</commit_message>
<xml_diff>
--- a/docs/Participant_tracker.xlsx
+++ b/docs/Participant_tracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kirill\Documents\Study\_RESEARCH\prof. Rosa\CNB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kirill\Documents\Study\_RESEARCH\prof. Rosa\CNB\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0EC6CA-89FC-43FE-BE8F-88E1B618D718}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BA1213-0AAC-46ED-BDA0-911D1E49BC51}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{70004516-9C23-4383-B67A-DD25032375F5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>1</t>
   </si>
@@ -92,12 +92,6 @@
     <t>SUBJECT</t>
   </si>
   <si>
-    <t xml:space="preserve">Consent </t>
-  </si>
-  <si>
-    <t>received</t>
-  </si>
-  <si>
     <t>Instruction</t>
   </si>
   <si>
@@ -135,6 +129,9 @@
   </si>
   <si>
     <t>Copy patient info</t>
+  </si>
+  <si>
+    <t>Consent received</t>
   </si>
 </sst>
 </file>
@@ -169,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -177,19 +174,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,65 +573,68 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.21875" customWidth="1"/>
-    <col min="2" max="9" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="9" width="10.109375" customWidth="1"/>
     <col min="10" max="16" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="L2" t="s">
@@ -610,79 +654,223 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>